<commit_message>
JGA example excel modified
</commit_message>
<xml_diff>
--- a/example/JSUB999999_jga_metadata.xlsx
+++ b/example/JSUB999999_jga_metadata.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28025"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637788CA-CF00-454D-B649-DF167018EA65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F89992-0A34-4EAF-8EF5-3EB0119666C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1055" uniqueCount="888">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1058" uniqueCount="891">
   <si>
     <t>E-mail</t>
     <phoneticPr fontId="1"/>
@@ -4530,6 +4530,16 @@
       <t>フカ</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Library Source SINGLE CELL</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>GENOMIC SINGLE CELL</t>
+  </si>
+  <si>
+    <t>TRANSCRIPTOMIC SINGLE CELL</t>
   </si>
 </sst>
 </file>
@@ -5089,7 +5099,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B46"/>
+  <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
@@ -5219,7 +5229,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.5">
       <c r="A28" s="7">
-        <v>45478</v>
+        <v>45588</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.5">
@@ -5353,6 +5363,14 @@
       </c>
       <c r="B46" s="7">
         <v>45478</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.5">
+      <c r="A47" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B47" s="7">
+        <v>45588</v>
       </c>
     </row>
   </sheetData>
@@ -5504,7 +5522,7 @@
         <v>245</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>272</v>
+        <v>889</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>279</v>
@@ -5551,7 +5569,7 @@
         <v>246</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>280</v>
@@ -5586,7 +5604,7 @@
         <v>247</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>274</v>
+        <v>890</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>281</v>
@@ -5621,7 +5639,7 @@
         <v>248</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>282</v>
@@ -5653,7 +5671,7 @@
         <v>249</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>283</v>
@@ -5685,7 +5703,7 @@
         <v>250</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>284</v>
@@ -5716,6 +5734,9 @@
       <c r="B9" s="1" t="s">
         <v>251</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>276</v>
+      </c>
       <c r="D9" s="1" t="s">
         <v>285</v>
       </c>
@@ -5744,6 +5765,9 @@
       </c>
       <c r="B10" s="1" t="s">
         <v>252</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>277</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>286</v>
@@ -9234,7 +9258,7 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
-            <xm:f>Admin!$C$2:$C$8</xm:f>
+            <xm:f>Admin!$C$2:$C$10</xm:f>
           </x14:formula1>
           <xm:sqref>F3:F102</xm:sqref>
         </x14:dataValidation>

</xml_diff>